<commit_message>
modified:   Documentation/IGNITE/IGNITE-Budget.xlsx 	modified:   Documentation/IGNITE/IGNITE_ALMA.pdf 	deleted:    Documentation/Nonlinear-FBL-Dynamics.pdf 	deleted:    Documentation/Philanthropy/Grant_Proposal.pdf 	deleted:    Documentation/Seed Laser Driver Pump Laser Diode Driver Fiber Laser Driver AMI - 762.pdf 	deleted:    Documentation/seed-diode.pdf 	Documentation/IGNITE/Budget&roster.odt 	Documentation/IGNITE/Budget-Roster.pdf 	Documentation/IGNITE/ERAU UNIVERSITY INTERNAL RESEARCH AWARDS - Ignite Grant RFP 2023-2024.pdf 	Documentation/IGNITE/FINAL-IGNITE-GRANT.pdf 	Documentation/IGNITE/IGNITE_ALMA_FULL.pdf 	Documentation/IGNITE/Jacob reference letter Ignite.pdf 	Documentation/IGNITE/Romeo_TItle Page.pdf 	Documentation/IGNITE/Title Page-Sig.odt 	Documentation/IGNITE/budget.png 	Documentation/IGNITE/summary.odt 	Documentation/IGNITE/title page.odt 	Documentation/Manuals/ 	Documentation/Papers/ 	Documentation/Philanthropy/Philanthropy_Grant_Proposal.pdf
</commit_message>
<xml_diff>
--- a/Documentation/IGNITE/IGNITE-Budget.xlsx
+++ b/Documentation/IGNITE/IGNITE-Budget.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t xml:space="preserve">Please click here to review the OUR Purchasing Guidelines prior to completing this form.</t>
   </si>
@@ -494,7 +494,7 @@
     <t xml:space="preserve">Lumics</t>
   </si>
   <si>
-    <t xml:space="preserve">BTF FBL module</t>
+    <t xml:space="preserve">BTF LASER diode</t>
   </si>
   <si>
     <t xml:space="preserve">LU0975M500</t>
@@ -506,19 +506,22 @@
     <t xml:space="preserve">Analog Modules</t>
   </si>
   <si>
-    <t xml:space="preserve">Control board</t>
+    <t xml:space="preserve">Seed diode Control board</t>
   </si>
   <si>
     <t xml:space="preserve">Model 762</t>
   </si>
   <si>
-    <t xml:space="preserve">TBD</t>
+    <t xml:space="preserve">Fibercore</t>
   </si>
   <si>
     <t xml:space="preserve">Yb doped fiber cable</t>
   </si>
   <si>
-    <t xml:space="preserve">Same as cable</t>
+    <t xml:space="preserve">custom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technica</t>
   </si>
   <si>
     <t xml:space="preserve">High reflectivity Fiber bragg grating</t>
@@ -527,6 +530,9 @@
     <t xml:space="preserve">Low reflectivity Fiber bragg grating</t>
   </si>
   <si>
+    <t xml:space="preserve">Uline</t>
+  </si>
+  <si>
     <t xml:space="preserve">Welding screen (Also getting a small one from SPARK)</t>
   </si>
   <si>
@@ -551,13 +557,85 @@
     <t xml:space="preserve">https://www.amazon.com/dp/B08XXN9TVN/ref=syn_sd_onsite_desktop_0?ie=UTF8&amp;pd_rd_plhdr=t&amp;th=1</t>
   </si>
   <si>
-    <t xml:space="preserve">Protective goggles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B09SHZXM1C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.amazon.com/Professional-740-1100nm-Protective-Industrial-Semi-Conductor/dp/B09SHZXM1C/ref=asc_df_B09SHZXM1C/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=598347691859&amp;hvpos=&amp;hvnetw=g&amp;hvrand=16691468661394200725&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9011497&amp;hvtargid=pla-2005947712752&amp;psc=1</t>
+    <t xml:space="preserve">pelican case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H-6800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.uline.com/Product/Detail/H-6800/Special-Use-Boxes/Pelican-1200-Equipment-Case?pricode=WB0026&amp;gadtype=pla&amp;id=H-6800&amp;gclid=CjwKCAiAr4GgBhBFEiwAgwORrZ4a8mueCDYfsj6qmGPA4-bIjYi8f_B3KQwXmyw64aeylFWCXTJ0RhoC3L8QAvD_BwE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO Photonics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spectrometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB4000-FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.gophotonics.com/products/spectrometers/ocean-optics-inc/44-543-usb4000-fl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocean Insight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fiber Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P200-1-VIS-NIR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for the spectrometer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.oceaninsight.com/products/fibers-and-probes/fibers/patch-cords/p200-1-vis-nir/?qty=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FTDI chip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART → USB-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TTL-232R-5V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ftdichip.com/products/ttl-232r-5v/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nilight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B099S866XH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To toggle power of apparatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.amazon.com/Nilight-90014E-Rocker-Toggle-Warranty/dp/B099S866XH/ref=asc_df_B07QKFD7Z7/?tag=&amp;linkCode=df0&amp;hvadid=362768105905&amp;hvpos=&amp;hvnetw=g&amp;hvrand=3797130617371782147&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9011497&amp;hvtargid=pla-784404092761&amp;ref=&amp;adgrpid=75266506039&amp;th=1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen Supplies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All equipment will be re-usable if not defected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gen equipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">everything</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer equip and soft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the control board comes with software needed</t>
   </si>
   <si>
     <r>
@@ -1490,7 +1568,7 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1666,6 +1744,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="26" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -1874,9 +1956,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>9000</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1235880</xdr:rowOff>
+      <xdr:rowOff>1234440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1890,7 +1972,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10440" y="0"/>
-          <a:ext cx="21078360" cy="1235880"/>
+          <a:ext cx="21076920" cy="1234440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1911,9 +1993,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1293120</xdr:colOff>
+      <xdr:colOff>1291680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1204560</xdr:rowOff>
+      <xdr:rowOff>1203120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1923,7 +2005,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3198960" y="42480"/>
-          <a:ext cx="15539040" cy="1162080"/>
+          <a:ext cx="15537600" cy="1160640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1975,9 +2057,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>791640</xdr:colOff>
+      <xdr:colOff>790200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1236240</xdr:rowOff>
+      <xdr:rowOff>1234800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1991,7 +2073,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="745920" y="0"/>
-          <a:ext cx="2546280" cy="1236240"/>
+          <a:ext cx="2544840" cy="1234800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2031,7 +2113,7 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
@@ -2091,10 +2173,10 @@
   </sheetPr>
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="10" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="bottomLeft" activeCell="P20" activeCellId="0" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2221,15 +2303,14 @@
       </c>
       <c r="I8" s="24"/>
       <c r="J8" s="25" t="n">
-        <f aca="false">SUM('Purchase Request '!$J$11:$J$110)</f>
-        <v>0</v>
+        <v>7600</v>
       </c>
       <c r="K8" s="26" t="s">
         <v>19</v>
       </c>
       <c r="L8" s="25" t="n">
         <f aca="false">SUM('Purchase Request '!$K$11:$K$110)</f>
-        <v>6574</v>
+        <v>7571.78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2292,13 +2373,13 @@
         <v>1</v>
       </c>
       <c r="H11" s="39" t="n">
-        <v>2000</v>
+        <v>2175</v>
       </c>
       <c r="I11" s="39"/>
       <c r="J11" s="40"/>
       <c r="K11" s="41" t="n">
         <f aca="false">'Purchase Request '!$H11*'Purchase Request '!$G11+'Purchase Request '!$I11</f>
-        <v>2000</v>
+        <v>2175</v>
       </c>
       <c r="L11" s="42"/>
     </row>
@@ -2344,7 +2425,7 @@
         <v>40</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E13" s="36"/>
       <c r="F13" s="37" t="s">
@@ -2369,29 +2450,29 @@
         <v>4</v>
       </c>
       <c r="B14" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>39</v>
-      </c>
       <c r="E14" s="36"/>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="37" t="s">
         <v>35</v>
       </c>
       <c r="G14" s="38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="39" t="n">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="I14" s="39"/>
       <c r="J14" s="40"/>
       <c r="K14" s="41" t="n">
         <f aca="false">'Purchase Request '!$H14*'Purchase Request '!$G14+'Purchase Request '!$I14</f>
-        <v>900</v>
+        <v>250</v>
       </c>
       <c r="L14" s="42"/>
     </row>
@@ -2400,29 +2481,29 @@
         <v>5</v>
       </c>
       <c r="B15" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>39</v>
-      </c>
       <c r="E15" s="36"/>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="37" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="38" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" s="39" t="n">
-        <v>240</v>
+        <v>300</v>
       </c>
       <c r="I15" s="39"/>
       <c r="J15" s="40"/>
       <c r="K15" s="41" t="n">
         <f aca="false">'Purchase Request '!$H15*'Purchase Request '!$G15+'Purchase Request '!$I15</f>
-        <v>720</v>
+        <v>600</v>
       </c>
       <c r="L15" s="42"/>
     </row>
@@ -2430,17 +2511,20 @@
       <c r="A16" s="32" t="n">
         <v>6</v>
       </c>
+      <c r="B16" s="44" t="s">
+        <v>45</v>
+      </c>
       <c r="C16" s="33" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E16" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>49</v>
       </c>
       <c r="G16" s="38" t="n">
         <v>2</v>
@@ -2461,17 +2545,17 @@
         <v>7</v>
       </c>
       <c r="B17" s="33" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E17" s="36"/>
-      <c r="F17" s="44" t="s">
-        <v>51</v>
+      <c r="F17" s="45" t="s">
+        <v>53</v>
       </c>
       <c r="G17" s="38" t="n">
         <v>1</v>
@@ -2492,29 +2576,29 @@
         <v>8</v>
       </c>
       <c r="B18" s="33" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="36"/>
-      <c r="F18" s="44" t="s">
-        <v>54</v>
+      <c r="F18" s="45" t="s">
+        <v>56</v>
       </c>
       <c r="G18" s="38" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" s="39" t="n">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="I18" s="39"/>
       <c r="J18" s="40"/>
       <c r="K18" s="41" t="n">
-        <f aca="false">'Purchase Request '!$H18*'Purchase Request '!$G18+'Purchase Request '!$I18</f>
-        <v>159</v>
+        <f aca="false">'Purchase Request '!$H18*'Purchase Request '!$G18+'Purchase Request '!$I19</f>
+        <v>72</v>
       </c>
       <c r="L18" s="42"/>
     </row>
@@ -2522,18 +2606,30 @@
       <c r="A19" s="32" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="43"/>
+      <c r="B19" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="43" t="s">
+        <v>59</v>
+      </c>
       <c r="E19" s="36"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
+      <c r="F19" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="39" t="n">
+        <v>1500</v>
+      </c>
       <c r="I19" s="39"/>
       <c r="J19" s="40"/>
       <c r="K19" s="41" t="n">
-        <f aca="false">'Purchase Request '!$H19*'Purchase Request '!$G19+'Purchase Request '!$I19</f>
-        <v>0</v>
+        <f aca="false">'Purchase Request '!$H19*'Purchase Request '!$G19+'Purchase Request '!$I20</f>
+        <v>1500</v>
       </c>
       <c r="L19" s="42"/>
     </row>
@@ -2541,18 +2637,32 @@
       <c r="A20" s="32" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="39"/>
+      <c r="B20" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="39" t="n">
+        <v>144</v>
+      </c>
       <c r="I20" s="39"/>
       <c r="J20" s="40"/>
       <c r="K20" s="41" t="n">
-        <f aca="false">'Purchase Request '!$H20*'Purchase Request '!$G20+'Purchase Request '!$I20</f>
-        <v>0</v>
+        <f aca="false">'Purchase Request '!$H20*'Purchase Request '!$G20+'Purchase Request '!$I21</f>
+        <v>144</v>
       </c>
       <c r="L20" s="42"/>
     </row>
@@ -2560,18 +2670,30 @@
       <c r="A21" s="32" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="43"/>
+      <c r="B21" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>68</v>
+      </c>
       <c r="E21" s="36"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="39"/>
+      <c r="F21" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" s="39" t="n">
+        <v>23.4</v>
+      </c>
       <c r="I21" s="39"/>
       <c r="J21" s="39"/>
       <c r="K21" s="41" t="n">
-        <f aca="false">'Purchase Request '!$H21*'Purchase Request '!$G21+'Purchase Request '!$I21</f>
-        <v>0</v>
+        <f aca="false">'Purchase Request '!$H21*'Purchase Request '!$G21+'Purchase Request '!$I22</f>
+        <v>23.4</v>
       </c>
       <c r="L21" s="42"/>
     </row>
@@ -2579,18 +2701,32 @@
       <c r="A22" s="32" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
+      <c r="B22" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="H22" s="39" t="n">
+        <v>12.38</v>
+      </c>
       <c r="I22" s="39"/>
       <c r="J22" s="39"/>
       <c r="K22" s="41" t="n">
         <f aca="false">'Purchase Request '!$H22*'Purchase Request '!$G22+'Purchase Request '!$I22</f>
-        <v>0</v>
+        <v>12.38</v>
       </c>
       <c r="L22" s="42"/>
     </row>
@@ -2602,7 +2738,7 @@
       <c r="C23" s="34"/>
       <c r="D23" s="43"/>
       <c r="E23" s="36"/>
-      <c r="F23" s="44"/>
+      <c r="F23" s="45"/>
       <c r="G23" s="38"/>
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
@@ -2621,7 +2757,7 @@
       <c r="C24" s="34"/>
       <c r="D24" s="43"/>
       <c r="E24" s="36"/>
-      <c r="F24" s="44"/>
+      <c r="F24" s="45"/>
       <c r="G24" s="38"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
@@ -2636,11 +2772,15 @@
       <c r="A25" s="32" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="34"/>
+      <c r="B25" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>76</v>
+      </c>
       <c r="D25" s="43"/>
       <c r="E25" s="36"/>
-      <c r="F25" s="44"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="38"/>
       <c r="H25" s="39"/>
       <c r="I25" s="39"/>
@@ -2658,11 +2798,15 @@
       <c r="A26" s="32" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
+      <c r="B26" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>78</v>
+      </c>
       <c r="D26" s="43"/>
       <c r="E26" s="36"/>
-      <c r="F26" s="44"/>
+      <c r="F26" s="45"/>
       <c r="G26" s="38"/>
       <c r="H26" s="39"/>
       <c r="I26" s="39"/>
@@ -2680,11 +2824,15 @@
       <c r="A27" s="32" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="34"/>
+      <c r="B27" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="D27" s="43"/>
       <c r="E27" s="36"/>
-      <c r="F27" s="44"/>
+      <c r="F27" s="45"/>
       <c r="G27" s="38"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39"/>
@@ -2706,7 +2854,7 @@
       <c r="C28" s="34"/>
       <c r="D28" s="43"/>
       <c r="E28" s="36"/>
-      <c r="F28" s="44"/>
+      <c r="F28" s="45"/>
       <c r="G28" s="38"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39"/>
@@ -2728,7 +2876,7 @@
       <c r="C29" s="34"/>
       <c r="D29" s="43"/>
       <c r="E29" s="36"/>
-      <c r="F29" s="44"/>
+      <c r="F29" s="45"/>
       <c r="G29" s="38"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39"/>
@@ -2750,7 +2898,7 @@
       <c r="C30" s="34"/>
       <c r="D30" s="43"/>
       <c r="E30" s="36"/>
-      <c r="F30" s="44"/>
+      <c r="F30" s="45"/>
       <c r="G30" s="38"/>
       <c r="H30" s="39"/>
       <c r="I30" s="39"/>
@@ -2772,7 +2920,7 @@
       <c r="C31" s="34"/>
       <c r="D31" s="43"/>
       <c r="E31" s="36"/>
-      <c r="F31" s="44"/>
+      <c r="F31" s="45"/>
       <c r="G31" s="38"/>
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
@@ -2794,7 +2942,7 @@
       <c r="C32" s="34"/>
       <c r="D32" s="43"/>
       <c r="E32" s="36"/>
-      <c r="F32" s="44"/>
+      <c r="F32" s="45"/>
       <c r="G32" s="38"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39"/>
@@ -2816,7 +2964,7 @@
       <c r="C33" s="34"/>
       <c r="D33" s="43"/>
       <c r="E33" s="36"/>
-      <c r="F33" s="44"/>
+      <c r="F33" s="45"/>
       <c r="G33" s="38"/>
       <c r="H33" s="39"/>
       <c r="I33" s="39"/>
@@ -2838,7 +2986,7 @@
       <c r="C34" s="34"/>
       <c r="D34" s="43"/>
       <c r="E34" s="36"/>
-      <c r="F34" s="44"/>
+      <c r="F34" s="45"/>
       <c r="G34" s="38"/>
       <c r="H34" s="39"/>
       <c r="I34" s="39"/>
@@ -2860,7 +3008,7 @@
       <c r="C35" s="34"/>
       <c r="D35" s="43"/>
       <c r="E35" s="36"/>
-      <c r="F35" s="44"/>
+      <c r="F35" s="45"/>
       <c r="G35" s="38"/>
       <c r="H35" s="39"/>
       <c r="I35" s="39"/>
@@ -2882,7 +3030,7 @@
       <c r="C36" s="34"/>
       <c r="D36" s="43"/>
       <c r="E36" s="36"/>
-      <c r="F36" s="44"/>
+      <c r="F36" s="45"/>
       <c r="G36" s="38"/>
       <c r="H36" s="39"/>
       <c r="I36" s="39"/>
@@ -2904,7 +3052,7 @@
       <c r="C37" s="34"/>
       <c r="D37" s="43"/>
       <c r="E37" s="36"/>
-      <c r="F37" s="44"/>
+      <c r="F37" s="45"/>
       <c r="G37" s="38"/>
       <c r="H37" s="39"/>
       <c r="I37" s="39"/>
@@ -2926,7 +3074,7 @@
       <c r="C38" s="34"/>
       <c r="D38" s="43"/>
       <c r="E38" s="36"/>
-      <c r="F38" s="44"/>
+      <c r="F38" s="45"/>
       <c r="G38" s="38"/>
       <c r="H38" s="39"/>
       <c r="I38" s="39"/>
@@ -2948,7 +3096,7 @@
       <c r="C39" s="34"/>
       <c r="D39" s="43"/>
       <c r="E39" s="36"/>
-      <c r="F39" s="44"/>
+      <c r="F39" s="45"/>
       <c r="G39" s="38"/>
       <c r="H39" s="39"/>
       <c r="I39" s="39"/>
@@ -2970,7 +3118,7 @@
       <c r="C40" s="34"/>
       <c r="D40" s="43"/>
       <c r="E40" s="36"/>
-      <c r="F40" s="44"/>
+      <c r="F40" s="45"/>
       <c r="G40" s="38"/>
       <c r="H40" s="39"/>
       <c r="I40" s="39"/>
@@ -2992,7 +3140,7 @@
       <c r="C41" s="34"/>
       <c r="D41" s="43"/>
       <c r="E41" s="36"/>
-      <c r="F41" s="44"/>
+      <c r="F41" s="45"/>
       <c r="G41" s="38"/>
       <c r="H41" s="39"/>
       <c r="I41" s="39"/>
@@ -3014,7 +3162,7 @@
       <c r="C42" s="34"/>
       <c r="D42" s="43"/>
       <c r="E42" s="36"/>
-      <c r="F42" s="44"/>
+      <c r="F42" s="45"/>
       <c r="G42" s="38"/>
       <c r="H42" s="39"/>
       <c r="I42" s="39"/>
@@ -3036,7 +3184,7 @@
       <c r="C43" s="34"/>
       <c r="D43" s="43"/>
       <c r="E43" s="36"/>
-      <c r="F43" s="44"/>
+      <c r="F43" s="45"/>
       <c r="G43" s="38"/>
       <c r="H43" s="39"/>
       <c r="I43" s="39"/>
@@ -3058,7 +3206,7 @@
       <c r="C44" s="34"/>
       <c r="D44" s="43"/>
       <c r="E44" s="36"/>
-      <c r="F44" s="44"/>
+      <c r="F44" s="45"/>
       <c r="G44" s="38"/>
       <c r="H44" s="39"/>
       <c r="I44" s="39"/>
@@ -3080,7 +3228,7 @@
       <c r="C45" s="34"/>
       <c r="D45" s="43"/>
       <c r="E45" s="36"/>
-      <c r="F45" s="44"/>
+      <c r="F45" s="45"/>
       <c r="G45" s="38"/>
       <c r="H45" s="39"/>
       <c r="I45" s="39"/>
@@ -3102,7 +3250,7 @@
       <c r="C46" s="34"/>
       <c r="D46" s="43"/>
       <c r="E46" s="36"/>
-      <c r="F46" s="44"/>
+      <c r="F46" s="45"/>
       <c r="G46" s="38"/>
       <c r="H46" s="39"/>
       <c r="I46" s="39"/>
@@ -3124,7 +3272,7 @@
       <c r="C47" s="34"/>
       <c r="D47" s="43"/>
       <c r="E47" s="36"/>
-      <c r="F47" s="44"/>
+      <c r="F47" s="45"/>
       <c r="G47" s="38"/>
       <c r="H47" s="39"/>
       <c r="I47" s="39"/>
@@ -3146,7 +3294,7 @@
       <c r="C48" s="34"/>
       <c r="D48" s="43"/>
       <c r="E48" s="36"/>
-      <c r="F48" s="44"/>
+      <c r="F48" s="45"/>
       <c r="G48" s="38"/>
       <c r="H48" s="39"/>
       <c r="I48" s="39"/>
@@ -3168,7 +3316,7 @@
       <c r="C49" s="34"/>
       <c r="D49" s="43"/>
       <c r="E49" s="36"/>
-      <c r="F49" s="44"/>
+      <c r="F49" s="45"/>
       <c r="G49" s="38"/>
       <c r="H49" s="39"/>
       <c r="I49" s="39"/>
@@ -3190,7 +3338,7 @@
       <c r="C50" s="34"/>
       <c r="D50" s="43"/>
       <c r="E50" s="36"/>
-      <c r="F50" s="44"/>
+      <c r="F50" s="45"/>
       <c r="G50" s="38"/>
       <c r="H50" s="39"/>
       <c r="I50" s="39"/>
@@ -3212,7 +3360,7 @@
       <c r="C51" s="34"/>
       <c r="D51" s="43"/>
       <c r="E51" s="36"/>
-      <c r="F51" s="44"/>
+      <c r="F51" s="45"/>
       <c r="G51" s="38"/>
       <c r="H51" s="39"/>
       <c r="I51" s="39"/>
@@ -3234,7 +3382,7 @@
       <c r="C52" s="34"/>
       <c r="D52" s="43"/>
       <c r="E52" s="36"/>
-      <c r="F52" s="44"/>
+      <c r="F52" s="45"/>
       <c r="G52" s="38"/>
       <c r="H52" s="39"/>
       <c r="I52" s="39"/>
@@ -3256,7 +3404,7 @@
       <c r="C53" s="34"/>
       <c r="D53" s="43"/>
       <c r="E53" s="36"/>
-      <c r="F53" s="44"/>
+      <c r="F53" s="45"/>
       <c r="G53" s="38"/>
       <c r="H53" s="39"/>
       <c r="I53" s="39"/>
@@ -3278,7 +3426,7 @@
       <c r="C54" s="34"/>
       <c r="D54" s="43"/>
       <c r="E54" s="36"/>
-      <c r="F54" s="44"/>
+      <c r="F54" s="45"/>
       <c r="G54" s="38"/>
       <c r="H54" s="39"/>
       <c r="I54" s="39"/>
@@ -3300,7 +3448,7 @@
       <c r="C55" s="34"/>
       <c r="D55" s="43"/>
       <c r="E55" s="36"/>
-      <c r="F55" s="44"/>
+      <c r="F55" s="45"/>
       <c r="G55" s="38"/>
       <c r="H55" s="39"/>
       <c r="I55" s="39"/>
@@ -3322,7 +3470,7 @@
       <c r="C56" s="34"/>
       <c r="D56" s="43"/>
       <c r="E56" s="36"/>
-      <c r="F56" s="44"/>
+      <c r="F56" s="45"/>
       <c r="G56" s="38"/>
       <c r="H56" s="39"/>
       <c r="I56" s="39"/>
@@ -3344,7 +3492,7 @@
       <c r="C57" s="34"/>
       <c r="D57" s="43"/>
       <c r="E57" s="36"/>
-      <c r="F57" s="44"/>
+      <c r="F57" s="45"/>
       <c r="G57" s="38"/>
       <c r="H57" s="39"/>
       <c r="I57" s="39"/>
@@ -3366,7 +3514,7 @@
       <c r="C58" s="34"/>
       <c r="D58" s="43"/>
       <c r="E58" s="36"/>
-      <c r="F58" s="44"/>
+      <c r="F58" s="45"/>
       <c r="G58" s="38"/>
       <c r="H58" s="39"/>
       <c r="I58" s="39"/>
@@ -3388,7 +3536,7 @@
       <c r="C59" s="34"/>
       <c r="D59" s="43"/>
       <c r="E59" s="36"/>
-      <c r="F59" s="44"/>
+      <c r="F59" s="45"/>
       <c r="G59" s="38"/>
       <c r="H59" s="39"/>
       <c r="I59" s="39"/>
@@ -3410,7 +3558,7 @@
       <c r="C60" s="34"/>
       <c r="D60" s="43"/>
       <c r="E60" s="36"/>
-      <c r="F60" s="44"/>
+      <c r="F60" s="45"/>
       <c r="G60" s="38"/>
       <c r="H60" s="39"/>
       <c r="I60" s="39"/>
@@ -3432,7 +3580,7 @@
       <c r="C61" s="34"/>
       <c r="D61" s="43"/>
       <c r="E61" s="36"/>
-      <c r="F61" s="44"/>
+      <c r="F61" s="45"/>
       <c r="G61" s="38"/>
       <c r="H61" s="39"/>
       <c r="I61" s="39"/>
@@ -3454,7 +3602,7 @@
       <c r="C62" s="34"/>
       <c r="D62" s="43"/>
       <c r="E62" s="36"/>
-      <c r="F62" s="44"/>
+      <c r="F62" s="45"/>
       <c r="G62" s="38"/>
       <c r="H62" s="39"/>
       <c r="I62" s="39"/>
@@ -3476,7 +3624,7 @@
       <c r="C63" s="34"/>
       <c r="D63" s="43"/>
       <c r="E63" s="36"/>
-      <c r="F63" s="44"/>
+      <c r="F63" s="45"/>
       <c r="G63" s="38"/>
       <c r="H63" s="39"/>
       <c r="I63" s="39"/>
@@ -3498,7 +3646,7 @@
       <c r="C64" s="34"/>
       <c r="D64" s="43"/>
       <c r="E64" s="36"/>
-      <c r="F64" s="44"/>
+      <c r="F64" s="45"/>
       <c r="G64" s="38"/>
       <c r="H64" s="39"/>
       <c r="I64" s="39"/>
@@ -3520,7 +3668,7 @@
       <c r="C65" s="34"/>
       <c r="D65" s="43"/>
       <c r="E65" s="36"/>
-      <c r="F65" s="44"/>
+      <c r="F65" s="45"/>
       <c r="G65" s="38"/>
       <c r="H65" s="39"/>
       <c r="I65" s="39"/>
@@ -3542,7 +3690,7 @@
       <c r="C66" s="34"/>
       <c r="D66" s="43"/>
       <c r="E66" s="36"/>
-      <c r="F66" s="44"/>
+      <c r="F66" s="45"/>
       <c r="G66" s="38"/>
       <c r="H66" s="39"/>
       <c r="I66" s="39"/>
@@ -3564,7 +3712,7 @@
       <c r="C67" s="34"/>
       <c r="D67" s="43"/>
       <c r="E67" s="36"/>
-      <c r="F67" s="44"/>
+      <c r="F67" s="45"/>
       <c r="G67" s="38"/>
       <c r="H67" s="39"/>
       <c r="I67" s="39"/>
@@ -3586,7 +3734,7 @@
       <c r="C68" s="34"/>
       <c r="D68" s="43"/>
       <c r="E68" s="36"/>
-      <c r="F68" s="44"/>
+      <c r="F68" s="45"/>
       <c r="G68" s="38"/>
       <c r="H68" s="39"/>
       <c r="I68" s="39"/>
@@ -3608,7 +3756,7 @@
       <c r="C69" s="34"/>
       <c r="D69" s="43"/>
       <c r="E69" s="36"/>
-      <c r="F69" s="44"/>
+      <c r="F69" s="45"/>
       <c r="G69" s="38"/>
       <c r="H69" s="39"/>
       <c r="I69" s="39"/>
@@ -3630,7 +3778,7 @@
       <c r="C70" s="34"/>
       <c r="D70" s="43"/>
       <c r="E70" s="36"/>
-      <c r="F70" s="44"/>
+      <c r="F70" s="45"/>
       <c r="G70" s="38"/>
       <c r="H70" s="39"/>
       <c r="I70" s="39"/>
@@ -3652,7 +3800,7 @@
       <c r="C71" s="34"/>
       <c r="D71" s="43"/>
       <c r="E71" s="36"/>
-      <c r="F71" s="44"/>
+      <c r="F71" s="45"/>
       <c r="G71" s="38"/>
       <c r="H71" s="39"/>
       <c r="I71" s="39"/>
@@ -3674,7 +3822,7 @@
       <c r="C72" s="34"/>
       <c r="D72" s="43"/>
       <c r="E72" s="36"/>
-      <c r="F72" s="44"/>
+      <c r="F72" s="45"/>
       <c r="G72" s="38"/>
       <c r="H72" s="39"/>
       <c r="I72" s="39"/>
@@ -3696,7 +3844,7 @@
       <c r="C73" s="34"/>
       <c r="D73" s="43"/>
       <c r="E73" s="36"/>
-      <c r="F73" s="44"/>
+      <c r="F73" s="45"/>
       <c r="G73" s="38"/>
       <c r="H73" s="39"/>
       <c r="I73" s="39"/>
@@ -3718,7 +3866,7 @@
       <c r="C74" s="34"/>
       <c r="D74" s="43"/>
       <c r="E74" s="36"/>
-      <c r="F74" s="44"/>
+      <c r="F74" s="45"/>
       <c r="G74" s="38"/>
       <c r="H74" s="39"/>
       <c r="I74" s="39"/>
@@ -3740,7 +3888,7 @@
       <c r="C75" s="34"/>
       <c r="D75" s="43"/>
       <c r="E75" s="36"/>
-      <c r="F75" s="44"/>
+      <c r="F75" s="45"/>
       <c r="G75" s="38"/>
       <c r="H75" s="39"/>
       <c r="I75" s="39"/>
@@ -3762,7 +3910,7 @@
       <c r="C76" s="34"/>
       <c r="D76" s="43"/>
       <c r="E76" s="36"/>
-      <c r="F76" s="44"/>
+      <c r="F76" s="45"/>
       <c r="G76" s="38"/>
       <c r="H76" s="39"/>
       <c r="I76" s="39"/>
@@ -3784,7 +3932,7 @@
       <c r="C77" s="34"/>
       <c r="D77" s="43"/>
       <c r="E77" s="36"/>
-      <c r="F77" s="44"/>
+      <c r="F77" s="45"/>
       <c r="G77" s="38"/>
       <c r="H77" s="39"/>
       <c r="I77" s="39"/>
@@ -3806,7 +3954,7 @@
       <c r="C78" s="34"/>
       <c r="D78" s="43"/>
       <c r="E78" s="36"/>
-      <c r="F78" s="44"/>
+      <c r="F78" s="45"/>
       <c r="G78" s="38"/>
       <c r="H78" s="39"/>
       <c r="I78" s="39"/>
@@ -3828,7 +3976,7 @@
       <c r="C79" s="34"/>
       <c r="D79" s="43"/>
       <c r="E79" s="36"/>
-      <c r="F79" s="44"/>
+      <c r="F79" s="45"/>
       <c r="G79" s="38"/>
       <c r="H79" s="39"/>
       <c r="I79" s="39"/>
@@ -3850,7 +3998,7 @@
       <c r="C80" s="34"/>
       <c r="D80" s="43"/>
       <c r="E80" s="36"/>
-      <c r="F80" s="44"/>
+      <c r="F80" s="45"/>
       <c r="G80" s="38"/>
       <c r="H80" s="39"/>
       <c r="I80" s="39"/>
@@ -3872,7 +4020,7 @@
       <c r="C81" s="34"/>
       <c r="D81" s="43"/>
       <c r="E81" s="36"/>
-      <c r="F81" s="44"/>
+      <c r="F81" s="45"/>
       <c r="G81" s="38"/>
       <c r="H81" s="39"/>
       <c r="I81" s="39"/>
@@ -3894,7 +4042,7 @@
       <c r="C82" s="34"/>
       <c r="D82" s="43"/>
       <c r="E82" s="36"/>
-      <c r="F82" s="44"/>
+      <c r="F82" s="45"/>
       <c r="G82" s="38"/>
       <c r="H82" s="39"/>
       <c r="I82" s="39"/>
@@ -3916,7 +4064,7 @@
       <c r="C83" s="34"/>
       <c r="D83" s="43"/>
       <c r="E83" s="36"/>
-      <c r="F83" s="44"/>
+      <c r="F83" s="45"/>
       <c r="G83" s="38"/>
       <c r="H83" s="39"/>
       <c r="I83" s="39"/>
@@ -3938,7 +4086,7 @@
       <c r="C84" s="34"/>
       <c r="D84" s="43"/>
       <c r="E84" s="36"/>
-      <c r="F84" s="44"/>
+      <c r="F84" s="45"/>
       <c r="G84" s="38"/>
       <c r="H84" s="39"/>
       <c r="I84" s="39"/>
@@ -3960,7 +4108,7 @@
       <c r="C85" s="34"/>
       <c r="D85" s="43"/>
       <c r="E85" s="36"/>
-      <c r="F85" s="44"/>
+      <c r="F85" s="45"/>
       <c r="G85" s="38"/>
       <c r="H85" s="39"/>
       <c r="I85" s="39"/>
@@ -3982,7 +4130,7 @@
       <c r="C86" s="34"/>
       <c r="D86" s="43"/>
       <c r="E86" s="36"/>
-      <c r="F86" s="44"/>
+      <c r="F86" s="45"/>
       <c r="G86" s="38"/>
       <c r="H86" s="39"/>
       <c r="I86" s="39"/>
@@ -4004,7 +4152,7 @@
       <c r="C87" s="34"/>
       <c r="D87" s="43"/>
       <c r="E87" s="36"/>
-      <c r="F87" s="44"/>
+      <c r="F87" s="45"/>
       <c r="G87" s="38"/>
       <c r="H87" s="39"/>
       <c r="I87" s="39"/>
@@ -4026,7 +4174,7 @@
       <c r="C88" s="34"/>
       <c r="D88" s="43"/>
       <c r="E88" s="36"/>
-      <c r="F88" s="44"/>
+      <c r="F88" s="45"/>
       <c r="G88" s="38"/>
       <c r="H88" s="39"/>
       <c r="I88" s="39"/>
@@ -4048,7 +4196,7 @@
       <c r="C89" s="34"/>
       <c r="D89" s="43"/>
       <c r="E89" s="36"/>
-      <c r="F89" s="44"/>
+      <c r="F89" s="45"/>
       <c r="G89" s="38"/>
       <c r="H89" s="39"/>
       <c r="I89" s="39"/>
@@ -4070,7 +4218,7 @@
       <c r="C90" s="34"/>
       <c r="D90" s="43"/>
       <c r="E90" s="36"/>
-      <c r="F90" s="44"/>
+      <c r="F90" s="45"/>
       <c r="G90" s="38"/>
       <c r="H90" s="39"/>
       <c r="I90" s="39"/>
@@ -4092,7 +4240,7 @@
       <c r="C91" s="34"/>
       <c r="D91" s="43"/>
       <c r="E91" s="36"/>
-      <c r="F91" s="44"/>
+      <c r="F91" s="45"/>
       <c r="G91" s="38"/>
       <c r="H91" s="39"/>
       <c r="I91" s="39"/>
@@ -4114,7 +4262,7 @@
       <c r="C92" s="34"/>
       <c r="D92" s="43"/>
       <c r="E92" s="36"/>
-      <c r="F92" s="44"/>
+      <c r="F92" s="45"/>
       <c r="G92" s="38"/>
       <c r="H92" s="39"/>
       <c r="I92" s="39"/>
@@ -4136,7 +4284,7 @@
       <c r="C93" s="34"/>
       <c r="D93" s="43"/>
       <c r="E93" s="36"/>
-      <c r="F93" s="44"/>
+      <c r="F93" s="45"/>
       <c r="G93" s="38"/>
       <c r="H93" s="39"/>
       <c r="I93" s="39"/>
@@ -4158,7 +4306,7 @@
       <c r="C94" s="34"/>
       <c r="D94" s="43"/>
       <c r="E94" s="36"/>
-      <c r="F94" s="44"/>
+      <c r="F94" s="45"/>
       <c r="G94" s="38"/>
       <c r="H94" s="39"/>
       <c r="I94" s="39"/>
@@ -4180,7 +4328,7 @@
       <c r="C95" s="34"/>
       <c r="D95" s="43"/>
       <c r="E95" s="36"/>
-      <c r="F95" s="44"/>
+      <c r="F95" s="45"/>
       <c r="G95" s="38"/>
       <c r="H95" s="39"/>
       <c r="I95" s="39"/>
@@ -4202,7 +4350,7 @@
       <c r="C96" s="34"/>
       <c r="D96" s="43"/>
       <c r="E96" s="36"/>
-      <c r="F96" s="44"/>
+      <c r="F96" s="45"/>
       <c r="G96" s="38"/>
       <c r="H96" s="39"/>
       <c r="I96" s="39"/>
@@ -4224,7 +4372,7 @@
       <c r="C97" s="34"/>
       <c r="D97" s="43"/>
       <c r="E97" s="36"/>
-      <c r="F97" s="44"/>
+      <c r="F97" s="45"/>
       <c r="G97" s="38"/>
       <c r="H97" s="39"/>
       <c r="I97" s="39"/>
@@ -4246,7 +4394,7 @@
       <c r="C98" s="34"/>
       <c r="D98" s="43"/>
       <c r="E98" s="36"/>
-      <c r="F98" s="44"/>
+      <c r="F98" s="45"/>
       <c r="G98" s="38"/>
       <c r="H98" s="39"/>
       <c r="I98" s="39"/>
@@ -4268,7 +4416,7 @@
       <c r="C99" s="34"/>
       <c r="D99" s="43"/>
       <c r="E99" s="36"/>
-      <c r="F99" s="44"/>
+      <c r="F99" s="45"/>
       <c r="G99" s="38"/>
       <c r="H99" s="39"/>
       <c r="I99" s="39"/>
@@ -4290,7 +4438,7 @@
       <c r="C100" s="34"/>
       <c r="D100" s="43"/>
       <c r="E100" s="36"/>
-      <c r="F100" s="44"/>
+      <c r="F100" s="45"/>
       <c r="G100" s="38"/>
       <c r="H100" s="39"/>
       <c r="I100" s="39"/>
@@ -4312,7 +4460,7 @@
       <c r="C101" s="34"/>
       <c r="D101" s="43"/>
       <c r="E101" s="36"/>
-      <c r="F101" s="44"/>
+      <c r="F101" s="45"/>
       <c r="G101" s="38"/>
       <c r="H101" s="39"/>
       <c r="I101" s="39"/>
@@ -4334,7 +4482,7 @@
       <c r="C102" s="34"/>
       <c r="D102" s="43"/>
       <c r="E102" s="36"/>
-      <c r="F102" s="44"/>
+      <c r="F102" s="45"/>
       <c r="G102" s="38"/>
       <c r="H102" s="39"/>
       <c r="I102" s="39"/>
@@ -4356,7 +4504,7 @@
       <c r="C103" s="34"/>
       <c r="D103" s="43"/>
       <c r="E103" s="36"/>
-      <c r="F103" s="44"/>
+      <c r="F103" s="45"/>
       <c r="G103" s="38"/>
       <c r="H103" s="39"/>
       <c r="I103" s="39"/>
@@ -4378,7 +4526,7 @@
       <c r="C104" s="34"/>
       <c r="D104" s="43"/>
       <c r="E104" s="36"/>
-      <c r="F104" s="44"/>
+      <c r="F104" s="45"/>
       <c r="G104" s="38"/>
       <c r="H104" s="39"/>
       <c r="I104" s="39"/>
@@ -4400,7 +4548,7 @@
       <c r="C105" s="34"/>
       <c r="D105" s="43"/>
       <c r="E105" s="36"/>
-      <c r="F105" s="44"/>
+      <c r="F105" s="45"/>
       <c r="G105" s="38"/>
       <c r="H105" s="39"/>
       <c r="I105" s="39"/>
@@ -4422,7 +4570,7 @@
       <c r="C106" s="34"/>
       <c r="D106" s="43"/>
       <c r="E106" s="36"/>
-      <c r="F106" s="44"/>
+      <c r="F106" s="45"/>
       <c r="G106" s="38"/>
       <c r="H106" s="39"/>
       <c r="I106" s="39"/>
@@ -4444,7 +4592,7 @@
       <c r="C107" s="34"/>
       <c r="D107" s="43"/>
       <c r="E107" s="36"/>
-      <c r="F107" s="44"/>
+      <c r="F107" s="45"/>
       <c r="G107" s="38"/>
       <c r="H107" s="39"/>
       <c r="I107" s="39"/>
@@ -4466,7 +4614,7 @@
       <c r="C108" s="34"/>
       <c r="D108" s="43"/>
       <c r="E108" s="36"/>
-      <c r="F108" s="44"/>
+      <c r="F108" s="45"/>
       <c r="G108" s="38"/>
       <c r="H108" s="39"/>
       <c r="I108" s="39"/>
@@ -4488,7 +4636,7 @@
       <c r="C109" s="34"/>
       <c r="D109" s="43"/>
       <c r="E109" s="36"/>
-      <c r="F109" s="44"/>
+      <c r="F109" s="45"/>
       <c r="G109" s="38"/>
       <c r="H109" s="39"/>
       <c r="I109" s="39"/>
@@ -4503,14 +4651,14 @@
       <c r="L109" s="42"/>
     </row>
     <row r="110" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="45" t="n">
+      <c r="A110" s="46" t="n">
         <v>100</v>
       </c>
       <c r="B110" s="33"/>
       <c r="C110" s="34"/>
       <c r="D110" s="43"/>
       <c r="E110" s="36"/>
-      <c r="F110" s="44"/>
+      <c r="F110" s="45"/>
       <c r="G110" s="38"/>
       <c r="H110" s="39"/>
       <c r="I110" s="39"/>
@@ -4518,21 +4666,21 @@
         <f aca="false">'Purchase Request '!$H110*'Purchase Request '!$G110+'Purchase Request '!$I110</f>
         <v>0</v>
       </c>
-      <c r="K110" s="46" t="n">
+      <c r="K110" s="47" t="n">
         <f aca="false">'Purchase Request '!$H110*'Purchase Request '!$G110+'Purchase Request '!$I110</f>
         <v>0</v>
       </c>
-      <c r="L110" s="47"/>
+      <c r="L110" s="48"/>
     </row>
     <row r="111" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C111" s="48"/>
-      <c r="D111" s="48"/>
-      <c r="E111" s="48"/>
-      <c r="F111" s="49"/>
-      <c r="G111" s="48"/>
-      <c r="H111" s="48"/>
-      <c r="I111" s="48"/>
-      <c r="J111" s="48"/>
+      <c r="C111" s="49"/>
+      <c r="D111" s="49"/>
+      <c r="E111" s="49"/>
+      <c r="F111" s="50"/>
+      <c r="G111" s="49"/>
+      <c r="H111" s="49"/>
+      <c r="I111" s="49"/>
+      <c r="J111" s="49"/>
     </row>
     <row r="112" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4567,7 +4715,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Electronic items &amp; hazardous and chemical items require approval. Provide additional info on appropriate tab below. " showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C11:C15 C17:C110" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Electronic items &amp; hazardous and chemical items require approval. Provide additional info on appropriate tab below. " showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C11:C15 C17:C21 C23:C110" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4583,7 +4731,11 @@
   <hyperlinks>
     <hyperlink ref="F16" r:id="rId1" display="https://www.uline.com/Product/Detail/H-5179S8/Welding/Welding-Screen-6-x-8-Shade-8"/>
     <hyperlink ref="F17" r:id="rId2" display="https://www.amazon.com/dp/B08XXN9TVN/ref=syn_sd_onsite_desktop_0?ie=UTF8&amp;pd_rd_plhdr=t&amp;th=1"/>
-    <hyperlink ref="F18" r:id="rId3" display="https://www.amazon.com/Professional-740-1100nm-Protective-Industrial-Semi-Conductor/dp/B09SHZXM1C/ref=asc_df_B09SHZXM1C/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=598347691859&amp;hvpos=&amp;hvnetw=g&amp;hvrand=16691468661394200725&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9011497&amp;hvtargid=pla-2005947712752&amp;psc=1"/>
+    <hyperlink ref="F18" r:id="rId3" display="https://www.uline.com/Product/Detail/H-6800/Special-Use-Boxes/Pelican-1200-Equipment-Case?pricode=WB0026&amp;gadtype=pla&amp;id=H-6800&amp;gclid=CjwKCAiAr4GgBhBFEiwAgwORrZ4a8mueCDYfsj6qmGPA4-bIjYi8f_B3KQwXmyw64aeylFWCXTJ0RhoC3L8QAvD_BwE"/>
+    <hyperlink ref="F19" r:id="rId4" display="https://www.gophotonics.com/products/spectrometers/ocean-optics-inc/44-543-usb4000-fl"/>
+    <hyperlink ref="F20" r:id="rId5" display="https://www.oceaninsight.com/products/fibers-and-probes/fibers/patch-cords/p200-1-vis-nir/?qty=1"/>
+    <hyperlink ref="F21" r:id="rId6" display="https://ftdichip.com/products/ttl-232r-5v/"/>
+    <hyperlink ref="F22" r:id="rId7" display="https://www.amazon.com/Nilight-90014E-Rocker-Toggle-Warranty/dp/B099S866XH/ref=asc_df_B07QKFD7Z7/?tag=&amp;linkCode=df0&amp;hvadid=362768105905&amp;hvpos=&amp;hvnetw=g&amp;hvrand=3797130617371782147&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hvlocphy=9011497&amp;hvtargid=pla-784404092761&amp;ref=&amp;adgrpid=75266506039&amp;th=1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.4" right="0.4" top="0.4" bottom="0.4" header="0.511811023622047" footer="0.3"/>
@@ -4594,9 +4746,9 @@
     <firstHeader/>
     <firstFooter/>
   </headerFooter>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId8"/>
   <tableParts>
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4609,7 +4761,7 @@
   </sheetPr>
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
@@ -4623,170 +4775,170 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="50"/>
+      <c r="A1" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="51"/>
     </row>
     <row r="2" customFormat="false" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="52" t="s">
-        <v>57</v>
+      <c r="A2" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="53" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="53" t="n">
+      <c r="A3" s="54" t="n">
         <v>4</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>58</v>
+      <c r="B3" s="55" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="55" t="n">
+      <c r="A4" s="56" t="n">
         <v>5</v>
       </c>
-      <c r="B4" s="56" t="s">
-        <v>59</v>
+      <c r="B4" s="57" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="53" t="n">
+      <c r="A5" s="54" t="n">
         <v>7</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>60</v>
+      <c r="B5" s="55" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55" t="n">
+      <c r="A6" s="56" t="n">
         <v>9</v>
       </c>
-      <c r="B6" s="56" t="s">
-        <v>61</v>
+      <c r="B6" s="57" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="57"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="55"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55"/>
-      <c r="B12" s="56"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="57"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="53"/>
-      <c r="B13" s="54"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="55"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55"/>
-      <c r="B14" s="56"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="57"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="53"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="53"/>
-      <c r="B17" s="54"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="55"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55"/>
-      <c r="B18" s="56"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="57"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="53"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="55"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="55"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="57"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="53"/>
-      <c r="B23" s="54"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="55"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55"/>
-      <c r="B24" s="56"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="57"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="55"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55"/>
-      <c r="B26" s="56"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="57"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="53"/>
-      <c r="B27" s="54"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="55"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="57"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="55"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="55"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="56"/>
+      <c r="B30" s="57"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="55"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="56"/>
+      <c r="B32" s="57"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="55"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="55"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="57"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="55"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="55"/>
-      <c r="B36" s="56"/>
+      <c r="A36" s="56"/>
+      <c r="B36" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4816,7 +4968,7 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -4832,230 +4984,230 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" customFormat="false" ht="63" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>65</v>
+      <c r="A2" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="53"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="55"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="53"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="55"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
+      <c r="A6" s="56"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="53"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="55"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="53"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
+      <c r="A9" s="54"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="55"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="53"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
+      <c r="A11" s="54"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="55"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="53"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
+      <c r="A13" s="54"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="55"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="62"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="53"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="55"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="53"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
+      <c r="A17" s="54"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="55"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="53"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="55"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="55"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="53"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="61"/>
+      <c r="A23" s="54"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="55"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
+      <c r="A24" s="56"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="53"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="55"/>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
+      <c r="A26" s="56"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="53"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
+      <c r="A27" s="54"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="55"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
+      <c r="A28" s="56"/>
+      <c r="B28" s="63"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="63"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="53"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
+      <c r="A29" s="54"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="55"/>
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
+      <c r="A30" s="56"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="53"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="55"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
+      <c r="A32" s="56"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="63"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="53"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
+      <c r="A33" s="54"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="55"/>
-      <c r="B34" s="62"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
+      <c r="A34" s="56"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="53"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
+      <c r="A35" s="54"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="55"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="62"/>
+      <c r="A36" s="56"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>